<commit_message>
Added new tier for zero tokens
</commit_message>
<xml_diff>
--- a/Cost of Bot.xlsx
+++ b/Cost of Bot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Italiandogs\Documents\Git-Repos\age-verifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC372C4-A733-40D0-B74A-68A43840DB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49BC3AC-D85F-4449-BA7C-DC14ED2563E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38460" yWindow="2160" windowWidth="21810" windowHeight="15435" xr2:uid="{D7E36C6D-CE28-40BE-9838-1C4AE6AF6DE5}"/>
+    <workbookView xWindow="8910" yWindow="3405" windowWidth="21810" windowHeight="15435" xr2:uid="{D7E36C6D-CE28-40BE-9838-1C4AE6AF6DE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -201,7 +202,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -212,6 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -549,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E7196C-04AE-436D-A0A5-F11A4B40A0ED}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,185 +1134,215 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" ref="D23" si="11">C23*B23</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2">
+        <f>E23-D23</f>
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
+        <f>F23*12</f>
+        <v>60</v>
+      </c>
+      <c r="H23" s="1" t="e">
+        <f>(E23-D23)/D23</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <f>10</f>
         <v>10</v>
       </c>
-      <c r="C23" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D23" s="2">
-        <f>C23*B23</f>
+      <c r="C24" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" ref="D24:D29" si="12">C24*B24</f>
         <v>15</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E24" s="5">
         <v>35</v>
       </c>
-      <c r="F23" s="2">
-        <f>E23-D23</f>
+      <c r="F24" s="2">
+        <f>E24-D24</f>
         <v>20</v>
       </c>
-      <c r="G23" s="2">
-        <f>F23*12</f>
+      <c r="G24" s="2">
+        <f>F24*12</f>
         <v>240</v>
       </c>
-      <c r="H23" s="1">
-        <f>(E23-D23)/D23</f>
+      <c r="H24" s="1">
+        <f>(E24-D24)/D24</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>2</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f>25</f>
         <v>25</v>
       </c>
-      <c r="C24" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D24" s="2">
-        <f>C24*B24</f>
+      <c r="C25" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="12"/>
         <v>37.5</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E25" s="5">
         <v>60</v>
       </c>
-      <c r="F24" s="2">
-        <f t="shared" ref="F24:F27" si="11">E24-D24</f>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:F28" si="13">E25-D25</f>
         <v>22.5</v>
       </c>
-      <c r="G24" s="2">
-        <f t="shared" ref="G24:G28" si="12">F24*12</f>
+      <c r="G25" s="2">
+        <f t="shared" ref="G25:G29" si="14">F25*12</f>
         <v>270</v>
       </c>
-      <c r="H24" s="1">
-        <f t="shared" ref="H24:H28" si="13">(E24-D24)/D24</f>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H29" si="15">(E25-D25)/D25</f>
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D25" s="2">
-        <f>C25*B25</f>
-        <v>75</v>
-      </c>
-      <c r="E25" s="5">
-        <v>85</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="11"/>
-        <v>10</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="12"/>
-        <v>120</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="13"/>
-        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="E26" s="5">
+        <v>85</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="14"/>
+        <v>120</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="15"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>4</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <f>75</f>
         <v>75</v>
       </c>
-      <c r="C26" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D26" s="2">
-        <f>C26*B26</f>
+      <c r="C27" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="12"/>
         <v>112.5</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E27" s="5">
         <v>135</v>
       </c>
-      <c r="F26" s="2">
-        <f t="shared" si="11"/>
+      <c r="F27" s="2">
+        <f t="shared" si="13"/>
         <v>22.5</v>
       </c>
-      <c r="G26" s="2">
-        <f t="shared" si="12"/>
+      <c r="G27" s="2">
+        <f t="shared" si="14"/>
         <v>270</v>
       </c>
-      <c r="H26" s="1">
-        <f t="shared" si="13"/>
+      <c r="H27" s="1">
+        <f t="shared" si="15"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>5</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="C27" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="2">
-        <f>C27*B27</f>
+      <c r="C28" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="12"/>
         <v>150</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E28" s="5">
         <v>175</v>
       </c>
-      <c r="F27" s="2">
-        <f t="shared" si="11"/>
+      <c r="F28" s="2">
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G28" s="2">
+        <f t="shared" si="14"/>
+        <v>300</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="15"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>150</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D29" s="2">
         <f t="shared" si="12"/>
-        <v>300</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="13"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28">
-        <v>150</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D28" s="2">
-        <f>C28*B28</f>
         <v>225</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E29" s="5">
         <v>275</v>
       </c>
-      <c r="F28" s="2">
-        <f>E28-D28</f>
+      <c r="F29" s="2">
+        <f>E29-D29</f>
         <v>50</v>
       </c>
-      <c r="G28" s="2">
-        <f t="shared" si="12"/>
+      <c r="G29" s="2">
+        <f t="shared" si="14"/>
         <v>600</v>
       </c>
-      <c r="H28" s="1">
-        <f t="shared" si="13"/>
+      <c r="H29" s="1">
+        <f t="shared" si="15"/>
         <v>0.22222222222222221</v>
       </c>
     </row>
@@ -1339,175 +1371,203 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="D32" s="6">
+        <f>B32-(D23*6)</f>
+        <v>30</v>
+      </c>
+      <c r="E32" s="6">
+        <f>C32-(D23*12)</f>
+        <v>60</v>
+      </c>
+      <c r="F32" s="1" t="e">
+        <f>(B32-(D23*6))/(D23*6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G32" s="1" t="e">
+        <f>(C32-(D23*12))/(D23*12)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>1</v>
       </c>
-      <c r="B32" s="6">
-        <f>(E23*6)/1.05</f>
+      <c r="B33" s="6">
+        <f>(E24*6)/1.05</f>
         <v>200</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C33" s="6">
         <f>380</f>
         <v>380</v>
       </c>
-      <c r="D32" s="6">
-        <f>B32-(D23*6)</f>
+      <c r="D33" s="6">
+        <f>B33-(D24*6)</f>
         <v>110</v>
       </c>
-      <c r="E32" s="6">
-        <f>C32-(D23*12)</f>
+      <c r="E33" s="6">
+        <f>C33-(D24*12)</f>
         <v>200</v>
       </c>
-      <c r="F32" s="1">
-        <f>(B32-(D23*6))/(D23*6)</f>
+      <c r="F33" s="1">
+        <f>(B33-(D24*6))/(D24*6)</f>
         <v>1.2222222222222223</v>
       </c>
-      <c r="G32" s="1">
-        <f>(C32-(D23*12))/(D23*12)</f>
+      <c r="G33" s="1">
+        <f>(C33-(D24*12))/(D24*12)</f>
         <v>1.1111111111111112</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>2</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B34" s="6">
         <f>345</f>
         <v>345</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C34" s="6">
         <f>655</f>
         <v>655</v>
       </c>
-      <c r="D33" s="6">
-        <f t="shared" ref="D33:D37" si="14">B33-(D24*6)</f>
+      <c r="D34" s="6">
+        <f>B34-(D25*6)</f>
         <v>120</v>
       </c>
-      <c r="E33" s="6">
-        <f t="shared" ref="E33:E37" si="15">C33-(D24*12)</f>
+      <c r="E34" s="6">
+        <f>C34-(D25*12)</f>
         <v>205</v>
       </c>
-      <c r="F33" s="1">
-        <f t="shared" ref="F33:F35" si="16">(B33-(D24*6))/(D24*6)</f>
+      <c r="F34" s="1">
+        <f>(B34-(D25*6))/(D25*6)</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="G33" s="1">
-        <f t="shared" ref="G33:G37" si="17">(C33-(D24*12))/(D24*12)</f>
+      <c r="G34" s="1">
+        <f>(C34-(D25*12))/(D25*12)</f>
         <v>0.45555555555555555</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>3</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B35" s="6">
         <f>490</f>
         <v>490</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C35" s="6">
         <f>930</f>
         <v>930</v>
       </c>
-      <c r="D34" s="6">
-        <f t="shared" si="14"/>
+      <c r="D35" s="6">
+        <f>B35-(D26*6)</f>
         <v>40</v>
       </c>
-      <c r="E34" s="6">
-        <f t="shared" si="15"/>
+      <c r="E35" s="6">
+        <f>C35-(D26*12)</f>
         <v>30</v>
       </c>
-      <c r="F34" s="1">
-        <f t="shared" si="16"/>
+      <c r="F35" s="1">
+        <f>(B35-(D26*6))/(D26*6)</f>
         <v>8.8888888888888892E-2</v>
       </c>
-      <c r="G34" s="1">
-        <f t="shared" si="17"/>
+      <c r="G35" s="1">
+        <f>(C35-(D26*12))/(D26*12)</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>4</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B36" s="6">
         <f>775</f>
         <v>775</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C36" s="6">
         <f>1475</f>
         <v>1475</v>
       </c>
-      <c r="D35" s="6">
-        <f t="shared" si="14"/>
+      <c r="D36" s="6">
+        <f>B36-(D27*6)</f>
         <v>100</v>
       </c>
-      <c r="E35" s="6">
-        <f t="shared" si="15"/>
+      <c r="E36" s="6">
+        <f>C36-(D27*12)</f>
         <v>125</v>
       </c>
-      <c r="F35" s="1">
-        <f t="shared" si="16"/>
+      <c r="F36" s="1">
+        <f>(B36-(D27*6))/(D27*6)</f>
         <v>0.14814814814814814</v>
       </c>
-      <c r="G35" s="1">
-        <f t="shared" si="17"/>
+      <c r="G36" s="1">
+        <f>(C36-(D27*12))/(D27*12)</f>
         <v>9.2592592592592587E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>5</v>
       </c>
-      <c r="B36" s="6">
-        <f t="shared" ref="B33:B37" si="18">(E27*6)/1.05</f>
+      <c r="B37" s="6">
+        <f>(E28*6)/1.05</f>
         <v>1000</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C37" s="6">
         <f>1910</f>
         <v>1910</v>
       </c>
-      <c r="D36" s="6">
-        <f t="shared" si="14"/>
+      <c r="D37" s="6">
+        <f>B37-(D28*6)</f>
         <v>100</v>
       </c>
-      <c r="E36" s="6">
-        <f t="shared" si="15"/>
+      <c r="E37" s="6">
+        <f>C37-(D28*12)</f>
         <v>110</v>
       </c>
-      <c r="F36" s="1">
-        <f>(B36-(D27*6))/(D27*6)</f>
+      <c r="F37" s="1">
+        <f>(B37-(D28*6))/(D28*6)</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="G36" s="1">
-        <f t="shared" si="17"/>
+      <c r="G37" s="1">
+        <f>(C37-(D28*12))/(D28*12)</f>
         <v>6.1111111111111109E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>6</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B38" s="6">
         <f>1575</f>
         <v>1575</v>
       </c>
-      <c r="C37" s="6">
-        <f t="shared" ref="C33:C37" si="19">(E28*12)/1.1</f>
+      <c r="C38" s="6">
+        <f>(E29*12)/1.1</f>
         <v>2999.9999999999995</v>
       </c>
-      <c r="D37" s="6">
-        <f t="shared" si="14"/>
+      <c r="D38" s="6">
+        <f>B38-(D29*6)</f>
         <v>225</v>
       </c>
-      <c r="E37" s="6">
-        <f t="shared" si="15"/>
+      <c r="E38" s="6">
+        <f>C38-(D29*12)</f>
         <v>299.99999999999955</v>
       </c>
-      <c r="F37" s="1">
-        <f>(B37-(D28*6))/(D28*6)</f>
+      <c r="F38" s="1">
+        <f>(B38-(D29*6))/(D29*6)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G37" s="1">
-        <f t="shared" si="17"/>
+      <c r="G38" s="1">
+        <f>(C38-(D29*12))/(D29*12)</f>
         <v>0.11111111111111094</v>
       </c>
     </row>

</xml_diff>